<commit_message>
Revisigng some functions like ROW, VLOOKUP, MATCH, INDEX
</commit_message>
<xml_diff>
--- a/VLOOKUP practice.xlsx
+++ b/VLOOKUP practice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\self projects\New folder\Documents\Exel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2EB5C2-0B4D-48BD-BF5C-3065E76AAB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7500B85D-1F86-4A8D-9F74-D114EA501C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{A4D4B17A-F7AB-4B0B-B1DE-A1482E48CE2F}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="10164" windowHeight="8964" xr2:uid="{A4D4B17A-F7AB-4B0B-B1DE-A1482E48CE2F}"/>
   </bookViews>
   <sheets>
     <sheet name="V-Lookup" sheetId="1" r:id="rId1"/>
@@ -455,10 +455,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +470,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -641,8 +647,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -650,7 +656,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -668,16 +674,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -685,6 +688,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40AA324-2AE2-42F3-B224-0A2C7460304B}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,7 +1038,7 @@
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1077,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="J2">
         <f>ROW()</f>
@@ -1105,11 +1109,11 @@
       </c>
       <c r="H3" s="18" t="str">
         <f>VLOOKUP($H$2,$A$1:$E$13, ROW()-1,0)</f>
-        <v>Employee_3</v>
+        <v>Employee_2</v>
       </c>
       <c r="I3" t="str">
         <f>VLOOKUP($H$2,$A$1:$E$13,ROW()-1,0)</f>
-        <v>Employee_3</v>
+        <v>Employee_2</v>
       </c>
       <c r="J3">
         <f>ROW()</f>
@@ -1140,7 +1144,7 @@
         <v>Operations</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I6" si="0">VLOOKUP($H$2,$A$1:$E$13,ROW()-1,0)</f>
+        <f t="shared" ref="I4:I5" si="0">VLOOKUP($H$2,$A$1:$E$13,ROW()-1,0)</f>
         <v>Operations</v>
       </c>
       <c r="J4">
@@ -1168,12 +1172,12 @@
         <v>3</v>
       </c>
       <c r="H5" s="18" t="str">
-        <f t="shared" ref="H4:H6" si="1">VLOOKUP($H$2,$A$1:$E$13, ROW()-1,0)</f>
-        <v>₹ 74,820.00</v>
+        <f t="shared" ref="H5" si="1">VLOOKUP($H$2,$A$1:$E$13, ROW()-1,0)</f>
+        <v>₹ 49,855.00</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>₹ 74,820.00</v>
+        <v>₹ 49,855.00</v>
       </c>
       <c r="J5">
         <f>ROW()</f>
@@ -1200,12 +1204,12 @@
         <v>4</v>
       </c>
       <c r="H6" s="18">
-        <f t="shared" si="1"/>
-        <v>43836</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>43836</v>
+        <f>VLOOKUP($H$2,$A$1:$E$13, ROW()-1,0)</f>
+        <v>43832</v>
+      </c>
+      <c r="I6" s="27">
+        <f>VLOOKUP($H$2,$A$1:$E$13,ROW()-1,0)</f>
+        <v>43832</v>
       </c>
       <c r="J6">
         <f>ROW()</f>
@@ -1351,6 +1355,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{4EF22263-FC2B-4F5D-A208-A41F5EB9EEC1}">
       <formula1>$A$2:$A$13</formula1>
@@ -1364,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B92B02-5332-437E-9EFE-3B647ECE5469}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="B1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1424,7 +1429,7 @@
         <f>VLOOKUP(D2, emp_type, 2, 1)</f>
         <v>Grade5</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="19" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="19" t="s">
@@ -1448,7 +1453,7 @@
         <v>43832</v>
       </c>
       <c r="F3" s="21" t="str">
-        <f>VLOOKUP(D3, emp_type, 2, 1)</f>
+        <f t="shared" ref="F2:F13" si="0">VLOOKUP(D3, emp_type, 2, 1)</f>
         <v>Grade4</v>
       </c>
       <c r="H3" s="23">
@@ -1475,7 +1480,7 @@
         <v>43833</v>
       </c>
       <c r="F4" s="21" t="str">
-        <f>VLOOKUP(D4, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade1</v>
       </c>
       <c r="H4" s="23">
@@ -1502,7 +1507,7 @@
         <v>43834</v>
       </c>
       <c r="F5" s="21" t="str">
-        <f>VLOOKUP(D5, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade3</v>
       </c>
       <c r="H5" s="23">
@@ -1529,7 +1534,7 @@
         <v>43835</v>
       </c>
       <c r="F6" s="21" t="str">
-        <f>VLOOKUP(D6, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade1</v>
       </c>
       <c r="H6" s="23">
@@ -1556,7 +1561,7 @@
         <v>43836</v>
       </c>
       <c r="F7" s="21" t="str">
-        <f>VLOOKUP(D7, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade3</v>
       </c>
       <c r="H7" s="23">
@@ -1583,7 +1588,7 @@
         <v>43837</v>
       </c>
       <c r="F8" s="21" t="str">
-        <f>VLOOKUP(D8, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade2</v>
       </c>
       <c r="H8" s="23">
@@ -1610,7 +1615,7 @@
         <v>43838</v>
       </c>
       <c r="F9" s="21" t="str">
-        <f>VLOOKUP(D9, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade5</v>
       </c>
     </row>
@@ -1631,7 +1636,7 @@
         <v>43839</v>
       </c>
       <c r="F10" s="21" t="str">
-        <f>VLOOKUP(D10, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade4</v>
       </c>
     </row>
@@ -1652,7 +1657,7 @@
         <v>43840</v>
       </c>
       <c r="F11" s="21" t="str">
-        <f>VLOOKUP(D11, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade5</v>
       </c>
     </row>
@@ -1673,7 +1678,7 @@
         <v>43841</v>
       </c>
       <c r="F12" s="21" t="str">
-        <f>VLOOKUP(D12, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade1</v>
       </c>
     </row>
@@ -1694,7 +1699,7 @@
         <v>43842</v>
       </c>
       <c r="F13" s="21" t="str">
-        <f>VLOOKUP(D13, emp_type, 2, 1)</f>
+        <f t="shared" si="0"/>
         <v>Grade2</v>
       </c>
     </row>
@@ -2028,34 +2033,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="26" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2317,7 +2322,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C12" t="s">

</xml_diff>